<commit_message>
Add data service for error codes and config variables
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="134">
   <si>
     <t>Name</t>
   </si>
@@ -421,6 +421,33 @@
   </si>
   <si>
     <t>NoReply</t>
+  </si>
+  <si>
+    <t>UseDB</t>
+  </si>
+  <si>
+    <t>Use auxiliary database for error codes and item data</t>
+  </si>
+  <si>
+    <t>UseDataServiceErrors</t>
+  </si>
+  <si>
+    <t>UseDataServiceItem</t>
+  </si>
+  <si>
+    <t>Use Data service for item data</t>
+  </si>
+  <si>
+    <t>Use Data service for error codes</t>
+  </si>
+  <si>
+    <t>ExceptionLanguage</t>
+  </si>
+  <si>
+    <t>EnforceSecondDataSource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If set to true, framework will attempt to get data from relevant data source (DB/Data Service). If data doesn't exist, an exception will be htrown . If false, it will not try to retrieve data from data source </t>
   </si>
 </sst>
 </file>
@@ -819,18 +846,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -887,7 +914,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="45">
+    <row r="4" spans="1:26" ht="43.5">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -897,7 +924,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="30">
+    <row r="6" spans="1:26" ht="29">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -908,129 +935,184 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.5">
+      <c r="B7" s="2"/>
+      <c r="C7" s="4"/>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" t="s">
-        <v>59</v>
+        <v>125</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="A11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="2"/>
+      <c r="A12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>101</v>
+      <c r="A13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B21" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B22" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="2" t="s">
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B23" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B24" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B18" s="8"/>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
         <v>102</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B26" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
         <v>104</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B28" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
         <v>113</v>
       </c>
-      <c r="B22" t="b">
+      <c r="B29" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2003,6 +2085,13 @@
     <row r="1002" ht="14.25" customHeight="1"/>
     <row r="1003" ht="14.25" customHeight="1"/>
     <row r="1004" ht="14.25" customHeight="1"/>
+    <row r="1005" ht="14.25" customHeight="1"/>
+    <row r="1006" ht="14.25" customHeight="1"/>
+    <row r="1007" ht="14.25" customHeight="1"/>
+    <row r="1008" ht="14.25" customHeight="1"/>
+    <row r="1009" ht="14.25" customHeight="1"/>
+    <row r="1010" ht="14.25" customHeight="1"/>
+    <row r="1011" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2018,12 +2107,12 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2060,7 +2149,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2071,7 +2160,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2185,7 +2274,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -3319,12 +3408,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -4408,12 +4497,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -5484,11 +5573,11 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Added rpaerrors schema for data service Fixed InitPaths Added option for Add Failed Items
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -448,6 +448,21 @@
   </si>
   <si>
     <t xml:space="preserve">If set to true, framework will attempt to get data from relevant data source (DB/Data Service). If data doesn't exist, an exception will be htrown . If false, it will not try to retrieve data from data source </t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Windows(\)</t>
+  </si>
+  <si>
+    <t>Unix(/)</t>
+  </si>
+  <si>
+    <t>Add failed items to next queue already as failed</t>
+  </si>
+  <si>
+    <t>AddFailedItem</t>
   </si>
 </sst>
 </file>
@@ -846,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1011"/>
+  <dimension ref="A1:Z1012"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -914,145 +929,148 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="43.5">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="43.5">
+      <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="29">
-      <c r="A6" t="s">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="29">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.5">
-      <c r="B7" s="2"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>126</v>
-      </c>
+    <row r="8" spans="1:26" ht="14.5">
+      <c r="B8" s="2"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>59</v>
+        <v>125</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>116</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B11" t="b">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
         <v>131</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" s="2" t="s">
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>101</v>
-      </c>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>101</v>
       </c>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>108</v>
+      <c r="A21" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>101</v>
@@ -1060,57 +1078,64 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>110</v>
+      <c r="A23" t="s">
+        <v>109</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" t="s">
-        <v>111</v>
+      <c r="A24" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B25" s="8"/>
+      <c r="A25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" t="s">
+      <c r="B26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
         <v>102</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
-        <v>104</v>
-      </c>
-      <c r="B28" t="s">
-        <v>105</v>
-      </c>
-    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
         <v>113</v>
       </c>
-      <c r="B29" t="b">
+      <c r="B30" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
@@ -2092,6 +2117,7 @@
     <row r="1009" ht="14.25" customHeight="1"/>
     <row r="1010" ht="14.25" customHeight="1"/>
     <row r="1011" ht="14.25" customHeight="1"/>
+    <row r="1012" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5567,20 +5593,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:AA998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.81640625" customWidth="1"/>
     <col min="2" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" customWidth="1"/>
+    <col min="5" max="27" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
+    <row r="1" spans="1:27" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5591,9 +5618,11 @@
         <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -5615,24 +5644,34 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA1" s="1"/>
+    </row>
+    <row r="2" spans="1:27" ht="14.25" customHeight="1">
+      <c r="D2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="14.25" customHeight="1">
+      <c r="D3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:27" ht="14.25" customHeight="1">
       <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:27" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:27" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -6616,6 +6655,11 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+      <formula1>"Windows(\),Unix(/)"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Test Cases, fixed minor bugs
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="141">
   <si>
     <t>Name</t>
   </si>
@@ -463,6 +463,12 @@
   </si>
   <si>
     <t>AddFailedItem</t>
+  </si>
+  <si>
+    <t>ErrorCodePath</t>
+  </si>
+  <si>
+    <t>Data\ErrorCodes.xlsx</t>
   </si>
 </sst>
 </file>
@@ -863,16 +869,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -940,7 +946,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="43.5">
+    <row r="5" spans="1:26" ht="45">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -950,7 +956,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="29">
+    <row r="7" spans="1:26" ht="30">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -961,7 +967,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.5">
+    <row r="8" spans="1:26">
       <c r="B8" s="2"/>
       <c r="C8" s="4"/>
     </row>
@@ -1000,7 +1006,7 @@
         <v>127</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>130</v>
@@ -1011,7 +1017,7 @@
         <v>128</v>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>129</v>
@@ -1022,7 +1028,7 @@
         <v>132</v>
       </c>
       <c r="B14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>133</v>
@@ -1133,10 +1139,17 @@
         <v>113</v>
       </c>
       <c r="B30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" t="s">
+        <v>140</v>
+      </c>
+    </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
@@ -2133,12 +2146,12 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2175,7 +2188,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2186,7 +2199,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2300,7 +2313,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -3434,12 +3447,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -4523,12 +4536,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -5599,12 +5612,12 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" customWidth="1"/>
-    <col min="5" max="27" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="27" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="14.25" customHeight="1">

</xml_diff>